<commit_message>
added GUI for portfolio mgmt
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">symbol</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entry_open</t>
   </si>
   <si>
     <t xml:space="preserve">TRIGYN</t>
@@ -144,13 +147,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="10.28"/>
@@ -172,10 +175,13 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>10</v>
@@ -189,10 +195,13 @@
       <c r="E2" s="0" t="n">
         <v>179</v>
       </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>10</v>
@@ -206,10 +215,13 @@
       <c r="E3" s="0" t="n">
         <v>355</v>
       </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>10</v>
@@ -222,6 +234,9 @@
       </c>
       <c r="E4" s="0" t="n">
         <v>70</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>